<commit_message>
Paso de usarse un array de niveles a usarse una tabla hash de niveles.
</commit_message>
<xml_diff>
--- a/nivelVacio.xlsx
+++ b/nivelVacio.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
   <si>
     <t>L</t>
   </si>
@@ -33,10 +33,13 @@
     <t>f</t>
   </si>
   <si>
+    <t>cv</t>
+  </si>
+  <si>
     <t>S</t>
   </si>
   <si>
-    <t>c</t>
+    <t>cp</t>
   </si>
   <si>
     <t>P</t>
@@ -343,7 +346,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="145" zoomScaleNormal="145" zoomScalePageLayoutView="100">
-      <selection activeCell="G7" activeCellId="0" pane="topLeft" sqref="G7"/>
+      <selection activeCell="E3" activeCellId="0" pane="topLeft" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <cols>
@@ -359,10 +362,10 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="1"/>
@@ -393,6 +396,9 @@
       <c r="A4" s="1" t="n">
         <v>5</v>
       </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C4" s="2"/>
       <c r="E4" s="2"/>
       <c r="G4" s="2"/>
@@ -404,10 +410,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J5" s="1"/>
     </row>
@@ -419,7 +422,7 @@
       <c r="E6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="1"/>
@@ -429,6 +432,9 @@
         <v>2</v>
       </c>
       <c r="C7" s="3"/>
+      <c r="E7" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="J7" s="1"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="8">
@@ -436,13 +442,13 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C8" s="2"/>
       <c r="E8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="1"/>
@@ -452,10 +458,10 @@
         <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>0</v>

</xml_diff>